<commit_message>
libiconv 1.14 => 1.15
git-svn-id: https://svn.nono303.net/build/msvc/httpd@2620 f19f5125-b473-6040-a4d2-80918b615817
</commit_message>
<xml_diff>
--- a/src-version.xlsx
+++ b/src-version.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\msvc.lan\c$\httpd-sdk\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nono\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{BD833ECE-66EE-4F35-8059-4033A0178AF6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{89E55D2D-551E-4F6A-9B71-7DB7345701CE}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19455" windowHeight="7635" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="version" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="102">
   <si>
     <t>https://github.com/apache/apr.git</t>
   </si>
@@ -86,9 +86,6 @@
   </si>
   <si>
     <t>R_2_2_5</t>
-  </si>
-  <si>
-    <t>https://github.com/LuaDist/libiconv</t>
   </si>
   <si>
     <t>https://github.com/GNOME/libxml2.git</t>
@@ -184,19 +181,6 @@
     <t>0327 OpenSSL_1_1_0g =&gt; OpenSSL_1_1_0h</t>
   </si>
   <si>
-    <t>7.2.4</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> * 0301
-0327 7.2.4</t>
-  </si>
-  <si>
-    <t>php-sdk-2.1.3beta1</t>
-  </si>
-  <si>
-    <t>0327 master =&gt; php-sdk-2.1.3beta1</t>
-  </si>
-  <si>
     <t>https://github.com/apache/subversion</t>
   </si>
   <si>
@@ -222,13 +206,6 @@
   </si>
   <si>
     <t>* 0328 - tag 1.3.9 KO (MSVC 14.1 existe pas)</t>
-  </si>
-  <si>
-    <t>0212 master =&gt; 1.10.16
-0410 1.10.17 =&gt; 1.10.17</t>
-  </si>
-  <si>
-    <t>1.10.17</t>
   </si>
   <si>
     <t>v1.0.4</t>
@@ -270,66 +247,100 @@
     <t>v1.31.1</t>
   </si>
   <si>
+    <t>msvc15 / msvc15-1.2.2</t>
+  </si>
+  <si>
+    <t>msvc15 / msvc15-1.6.1</t>
+  </si>
+  <si>
+    <t>msvc15 / msvc15-1.6.3</t>
+  </si>
+  <si>
+    <t>msvc15 / msvc15-master</t>
+  </si>
+  <si>
+    <t>msvc15 / msvc15-2.4.33</t>
+  </si>
+  <si>
+    <t>msvc15 / msvc15-4.3.1</t>
+  </si>
+  <si>
+    <t>msvc15 / msvc15-5.3.2</t>
+  </si>
+  <si>
+    <t>msvc15 / msvc15-1.1.0</t>
+  </si>
+  <si>
+    <t>msvc15 / msvc15-1.3.2</t>
+  </si>
+  <si>
+    <t>msvc15 / msvc15-2.9.8</t>
+  </si>
+  <si>
+    <t>msvc15 / msvc15-1.5.7</t>
+  </si>
+  <si>
+    <t>msvc15 / msvc15-OpenSSL_1_1_0h</t>
+  </si>
+  <si>
+    <t>msvc15 : bugfix</t>
+  </si>
+  <si>
+    <t>https://github.com/traceypooh/mod_h264_streaming--intra-keyframes.git</t>
+  </si>
+  <si>
+    <t>https://svn.nono303.net/code/wku_bt</t>
+  </si>
+  <si>
+    <t>msvc15 / msvc15-2.24-103</t>
+  </si>
+  <si>
+    <t>msvc15 / msvc15-NON_BLOCKING_IO_php7</t>
+  </si>
+  <si>
+    <t>msvc15 / msvc15-trunk</t>
+  </si>
+  <si>
+    <t>7.2.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> * 0301
+0327 7.2.4
+0425 7.2.5</t>
+  </si>
+  <si>
+    <t>1.10.20</t>
+  </si>
+  <si>
+    <t>0212 master =&gt; 1.10.16
+0410 1.10.17 =&gt; 1.10.17
+0502 1.10.20</t>
+  </si>
+  <si>
     <t>0206 master =&gt; v1.30.0
 0301 v1.30.0 =&gt; v1.31.0
-0415 v1.31.0 =&gt; v1.31.1</t>
-  </si>
-  <si>
-    <t>msvc15 / msvc15-1.2.2</t>
-  </si>
-  <si>
-    <t>msvc15 / msvc15-1.6.1</t>
-  </si>
-  <si>
-    <t>msvc15 / msvc15-1.6.3</t>
-  </si>
-  <si>
-    <t>msvc15 / msvc15-master</t>
-  </si>
-  <si>
-    <t>msvc15 / msvc15-2.4.33</t>
-  </si>
-  <si>
-    <t>msvc15 / msvc15-4.3.1</t>
-  </si>
-  <si>
-    <t>msvc15 / msvc15-5.3.2</t>
-  </si>
-  <si>
-    <t>msvc15 / msvc15-1.1.0</t>
-  </si>
-  <si>
-    <t>msvc15 / msvc15-1.3.2</t>
-  </si>
-  <si>
-    <t>msvc15 / msvc15-v1.31.1</t>
-  </si>
-  <si>
-    <t>msvc15 / msvc15-2.9.8</t>
-  </si>
-  <si>
-    <t>msvc15 / msvc15-1.5.7</t>
-  </si>
-  <si>
-    <t>msvc15 / msvc15-OpenSSL_1_1_0h</t>
-  </si>
-  <si>
-    <t>msvc15 : bugfix</t>
-  </si>
-  <si>
-    <t>https://github.com/traceypooh/mod_h264_streaming--intra-keyframes.git</t>
-  </si>
-  <si>
-    <t>https://svn.nono303.net/code/wku_bt</t>
-  </si>
-  <si>
-    <t>msvc15 / msvc15-2.24-103</t>
-  </si>
-  <si>
-    <t>msvc15 / msvc15-NON_BLOCKING_IO_php7</t>
-  </si>
-  <si>
-    <t>msvc15 / msvc15-trunk</t>
+0415 v1.31.0 =&gt; v1.31.1
+0514 v1.32.0</t>
+  </si>
+  <si>
+    <t>msvc15 / msvc15-v1.32.0</t>
+  </si>
+  <si>
+    <t>php-sdk-2.1.5</t>
+  </si>
+  <si>
+    <t>0327 master =&gt; php-sdk-2.1.3beta1
+0502 php-sdk-2.1.4
+0514 php-sdk-2.1.5</t>
+  </si>
+  <si>
+    <t>msvc15 / msvc15-1.15</t>
+  </si>
+  <si>
+    <t>https://github.com/kiyolee/libiconv-win-build</t>
+  </si>
+  <si>
+    <t>0515 : 1.14 https://github.com/LuaDist/libiconv =&gt; 1.15 https://github.com/kiyolee/libiconv-win-build</t>
   </si>
 </sst>
 </file>
@@ -472,7 +483,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="38">
+  <fills count="39">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -679,6 +690,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -862,9 +879,6 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -876,6 +890,9 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1233,8 +1250,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" topLeftCell="D4" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1242,48 +1259,48 @@
     <col min="1" max="1" width="68.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="78.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="112.42578125" customWidth="1"/>
+    <col min="5" max="5" width="92.85546875" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
-        <v>83</v>
+      <c r="B1" s="11" t="s">
+        <v>75</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="2"/>
-      <c r="E1" s="10"/>
+      <c r="E1" s="9"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="12" t="s">
-        <v>82</v>
+      <c r="B2" s="11" t="s">
+        <v>74</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="2"/>
-      <c r="E2" s="10"/>
+      <c r="E2" s="9"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>36</v>
-      </c>
       <c r="D3" s="2"/>
-      <c r="E3" s="10"/>
+      <c r="E3" s="9"/>
     </row>
     <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -1291,19 +1308,19 @@
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="3" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="E4" s="10"/>
+        <v>62</v>
+      </c>
+      <c r="E4" s="9"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="12" t="s">
-        <v>84</v>
+      <c r="B5" s="11" t="s">
+        <v>76</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>6</v>
@@ -1311,7 +1328,7 @@
       <c r="D5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="10"/>
+      <c r="E5" s="9"/>
     </row>
     <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
@@ -1322,24 +1339,24 @@
         <v>9</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="E6" s="10"/>
+        <v>41</v>
+      </c>
+      <c r="E6" s="9"/>
     </row>
     <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="12" t="s">
-        <v>85</v>
+      <c r="B7" s="11" t="s">
+        <v>77</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="E7" s="10"/>
+        <v>44</v>
+      </c>
+      <c r="E7" s="9"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
@@ -1352,14 +1369,14 @@
       <c r="D8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="10"/>
+      <c r="E8" s="9"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="12" t="s">
-        <v>86</v>
+      <c r="B9" s="11" t="s">
+        <v>78</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>15</v>
@@ -1367,7 +1384,7 @@
       <c r="D9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="10"/>
+      <c r="E9" s="9"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
@@ -1380,7 +1397,7 @@
       <c r="D10" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="10"/>
+      <c r="E10" s="9"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
@@ -1391,67 +1408,69 @@
         <v>21</v>
       </c>
       <c r="D11" s="2"/>
-      <c r="E11" s="10"/>
+      <c r="E11" s="9"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" s="2"/>
+      <c r="A12" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>99</v>
+      </c>
       <c r="C12" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E12" s="10"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="9" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
+      <c r="A13" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B13" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>50</v>
-      </c>
       <c r="D13" s="2"/>
-      <c r="E13" s="10"/>
+      <c r="E13" s="9"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14" s="12" t="s">
-        <v>91</v>
+        <v>22</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>82</v>
       </c>
       <c r="C14" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E14" s="10"/>
+      <c r="E14" s="9"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>25</v>
-      </c>
       <c r="D15" s="2"/>
-      <c r="E15" s="10"/>
+      <c r="E15" s="9"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B16" s="10"/>
+        <v>25</v>
+      </c>
+      <c r="B16" s="9"/>
       <c r="C16" s="2" t="s">
         <v>6</v>
       </c>
@@ -1459,104 +1478,104 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="10" t="s">
-        <v>27</v>
+    <row r="17" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
+        <v>26</v>
       </c>
       <c r="B17" s="6"/>
       <c r="C17" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="E17" s="10"/>
+        <v>93</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E17" s="9"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="B18" s="12" t="s">
-        <v>84</v>
+        <v>86</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>76</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D18" s="9"/>
-      <c r="E18" s="10" t="s">
-        <v>94</v>
+      <c r="D18" s="8"/>
+      <c r="E18" s="9" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="10" t="s">
+      <c r="A19" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B19" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>48</v>
-      </c>
       <c r="D19" s="2"/>
-      <c r="E19" s="10" t="s">
-        <v>94</v>
+      <c r="E19" s="9" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B20" s="6"/>
       <c r="C20" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D20" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="E20" s="10"/>
+      <c r="E20" s="9"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="12" t="s">
-        <v>96</v>
+      <c r="A21" s="11" t="s">
+        <v>87</v>
       </c>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
-      <c r="E21" s="10"/>
-    </row>
-    <row r="22" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="E21" s="9"/>
+    </row>
+    <row r="22" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B22" s="12" t="s">
-        <v>90</v>
+        <v>28</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>96</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="E22" s="10"/>
+        <v>95</v>
+      </c>
+      <c r="E22" s="9"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B23" s="12" t="s">
-        <v>93</v>
+        <v>29</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>84</v>
       </c>
       <c r="C23" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D23" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D23" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="E23" s="10"/>
+      <c r="E23" s="9"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" s="2" t="s">
@@ -1565,31 +1584,31 @@
       <c r="D24" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E24" s="10" t="s">
-        <v>37</v>
+      <c r="E24" s="9" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D25" s="2"/>
-      <c r="E25" s="10"/>
+      <c r="E25" s="9"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D26" s="2"/>
-      <c r="E26" s="10"/>
+      <c r="E26" s="9"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
@@ -1597,67 +1616,72 @@
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
     </row>
-    <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D28" s="8" t="s">
-        <v>54</v>
-      </c>
+        <v>91</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="E28" s="9"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D29" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D29" t="s">
-        <v>39</v>
-      </c>
+      <c r="E29" s="9"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B30" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="B30" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E30" s="9" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D31" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="C30" t="s">
-        <v>72</v>
-      </c>
-      <c r="D30" t="s">
-        <v>39</v>
-      </c>
-      <c r="E30" s="10" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B31" s="2"/>
-      <c r="C31" t="s">
-        <v>55</v>
-      </c>
-      <c r="D31" t="s">
-        <v>56</v>
-      </c>
+      <c r="E31" s="9"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="B32" s="2"/>
-      <c r="C32" t="s">
-        <v>74</v>
-      </c>
+      <c r="C32" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D32" s="2"/>
+      <c r="E32" s="9"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
@@ -1667,13 +1691,13 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B34" s="12" t="s">
-        <v>92</v>
+        <v>53</v>
+      </c>
+      <c r="B34" s="11" t="s">
+        <v>83</v>
       </c>
       <c r="C34" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -1684,38 +1708,38 @@
     </row>
     <row r="36" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" s="2" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>63</v>
-      </c>
-      <c r="B37" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="C37" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="D37" s="10" t="s">
-        <v>65</v>
+        <v>58</v>
+      </c>
+      <c r="B37" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D37" s="9" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="C38" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="D38" s="10"/>
+        <v>68</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="D38" s="9"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
@@ -1725,20 +1749,20 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="B40" s="12" t="s">
-        <v>97</v>
+        <v>64</v>
+      </c>
+      <c r="B40" s="11" t="s">
+        <v>88</v>
       </c>
       <c r="C40" t="s">
         <v>6</v>
       </c>
-      <c r="D40" s="11">
+      <c r="D40" s="10">
         <v>42871</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E44" s="13"/>
+      <c r="E44" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add freetype libpng libxpm change libiconv
git-svn-id: https://svn.nono303.net/build/msvc/httpd@2654 f19f5125-b473-6040-a4d2-80918b615817
</commit_message>
<xml_diff>
--- a/src-version.xlsx
+++ b/src-version.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="105">
   <si>
     <t>https://github.com/apache/apr.git</t>
   </si>
@@ -299,16 +299,6 @@
 0514 php-sdk-2.1.5</t>
   </si>
   <si>
-    <t>msvc15 / msvc15-1.15</t>
-  </si>
-  <si>
-    <t>https://github.com/kiyolee/libiconv-win-build</t>
-  </si>
-  <si>
-    <t>0515 : 1.14 https://github.com/LuaDist/libiconv =&gt; 1.15 https://github.com/kiyolee/libiconv-win-build
- - relocate include an vcxproj from https://github.com/holy-shit/iconv-for-windows.git</t>
-  </si>
-  <si>
     <t>msvc15 / msvc15-1.3.9</t>
   </si>
   <si>
@@ -343,13 +333,28 @@
 0327 7.2.4
 0425 7.2.5
 0612 7.2.6</t>
+  </si>
+  <si>
+    <t>https://github.com/winlibs/libiconv.git</t>
+  </si>
+  <si>
+    <t>https://github.com/winlibs/libpng.git</t>
+  </si>
+  <si>
+    <t>https://github.com/winlibs/libxpm</t>
+  </si>
+  <si>
+    <t>https://github.com/winlibs/freetype.git</t>
+  </si>
+  <si>
+    <t>0613 - master</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -484,8 +489,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="39">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -692,12 +705,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B0F0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -818,7 +825,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -861,6 +868,7 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -892,14 +900,14 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20 % - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20 % - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20 % - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -930,6 +938,7 @@
     <cellStyle name="Commentaire" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Entrée" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Insatisfaisant" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Lien hypertexte" xfId="42" builtinId="8"/>
     <cellStyle name="Neutre" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Satisfaisant" xfId="6" builtinId="26" customBuiltin="1"/>
@@ -1245,7 +1254,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1253,10 +1262,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E44"/>
+  <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33:XFD33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1377,7 +1386,7 @@
       <c r="E8" s="9"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="14" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="11" t="s">
@@ -1415,20 +1424,20 @@
       <c r="D11" s="2"/>
       <c r="E11" s="9"/>
     </row>
-    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="C12" s="2" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="C12" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="5"/>
-      <c r="E12" s="14" t="s">
-        <v>92</v>
-      </c>
+      <c r="D12" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E12" s="9"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
@@ -1532,10 +1541,10 @@
       </c>
       <c r="B20" s="6"/>
       <c r="C20" s="6" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E20" s="9"/>
     </row>
@@ -1627,10 +1636,10 @@
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E28" s="9"/>
     </row>
@@ -1689,90 +1698,138 @@
       <c r="E32" s="9"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="1"/>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
+      <c r="A33" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B33" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E33" s="9"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B34" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E34" s="9"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B35" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E35" s="9"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B34" s="11" t="s">
+      <c r="B37" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="C37" t="s">
+        <v>93</v>
+      </c>
+      <c r="D37" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="C34" t="s">
-        <v>96</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="1"/>
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-    </row>
-    <row r="36" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="1"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+    </row>
+    <row r="39" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B36" s="2"/>
-      <c r="C36" s="2" t="s">
+      <c r="B39" s="2"/>
+      <c r="C39" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D36" s="5" t="s">
+      <c r="D39" s="5" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+    <row r="40" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>56</v>
       </c>
-      <c r="B37" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="C37" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="D37" s="14" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="7" t="s">
+      <c r="B40" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="D40" s="13" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="C38" s="9" t="s">
+      <c r="C41" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="D38" s="9"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="1"/>
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
-      <c r="D39" s="1"/>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="7" t="s">
+      <c r="D41" s="9"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="1"/>
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="B40" s="11" t="s">
+      <c r="B43" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C43" t="s">
         <v>6</v>
       </c>
-      <c r="D40" s="10">
+      <c r="D43" s="10">
         <v>42871</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E44" s="12"/>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E47" s="12"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A9" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
move extracompile flags from sh to cmake opt add /arch:AVX for httpd xdebug 2.6.1
</commit_message>
<xml_diff>
--- a/src-version.xlsx
+++ b/src-version.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="109">
   <si>
     <t>https://github.com/apache/apr.git</t>
   </si>
@@ -122,9 +122,6 @@
   </si>
   <si>
     <t xml:space="preserve"> 8.41 with JIT, SUPPORT_UTF, SUPPORT_UNICODE_PROPERTIES, REBUILD_CHARTABLES </t>
-  </si>
-  <si>
-    <t>2.6.0</t>
   </si>
   <si>
     <t xml:space="preserve"> * 0301</t>
@@ -368,6 +365,13 @@
   </si>
   <si>
     <t>0724 : 3.24.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> * 0301
+0803 2.6.1</t>
+  </si>
+  <si>
+    <t>2.6.1</t>
   </si>
 </sst>
 </file>
@@ -1277,7 +1281,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1287,8 +1291,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1305,7 +1309,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>1</v>
@@ -1318,7 +1322,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>3</v>
@@ -1331,7 +1335,7 @@
         <v>33</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>34</v>
@@ -1345,10 +1349,10 @@
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>87</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>88</v>
       </c>
       <c r="E4" s="9"/>
     </row>
@@ -1357,7 +1361,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>6</v>
@@ -1373,10 +1377,10 @@
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E6" s="9"/>
     </row>
@@ -1385,13 +1389,13 @@
         <v>9</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E7" s="9"/>
     </row>
@@ -1413,7 +1417,7 @@
         <v>13</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>14</v>
@@ -1449,28 +1453,28 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>6</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E12" s="9"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>44</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="9"/>
@@ -1480,13 +1484,13 @@
         <v>21</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C14" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>39</v>
       </c>
       <c r="E14" s="9"/>
     </row>
@@ -1495,7 +1499,7 @@
         <v>22</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>23</v>
@@ -1521,41 +1525,41 @@
       </c>
       <c r="B17" s="6"/>
       <c r="C17" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="D17" s="8" t="s">
         <v>75</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>76</v>
       </c>
       <c r="E17" s="9"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D18" s="8"/>
       <c r="E18" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="B19" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>42</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1564,16 +1568,16 @@
       </c>
       <c r="B20" s="6"/>
       <c r="C20" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="D20" s="8" t="s">
         <v>89</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>90</v>
       </c>
       <c r="E20" s="9"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
@@ -1585,13 +1589,13 @@
         <v>27</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E22" s="9"/>
     </row>
@@ -1600,13 +1604,13 @@
         <v>28</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C23" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D23" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>46</v>
       </c>
       <c r="E23" s="9"/>
     </row>
@@ -1655,113 +1659,113 @@
     </row>
     <row r="28" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D28" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="D28" s="5" t="s">
-        <v>97</v>
-      </c>
       <c r="E28" s="9"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>37</v>
+        <v>108</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>107</v>
       </c>
       <c r="E29" s="9"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E31" s="9"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D32" s="2"/>
       <c r="E32" s="9"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C33" s="9" t="s">
         <v>6</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E33" s="9"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C34" s="9" t="s">
         <v>6</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E34" s="9"/>
     </row>
     <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B35" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="C35" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="C35" s="9" t="s">
-        <v>86</v>
-      </c>
       <c r="D35" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E35" s="9"/>
     </row>
@@ -1773,16 +1777,16 @@
     </row>
     <row r="37" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B37" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D37" s="5" t="s">
         <v>92</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="D37" s="5" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -1793,38 +1797,38 @@
     </row>
     <row r="39" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D39" s="5" t="s">
         <v>105</v>
-      </c>
-      <c r="D39" s="5" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B40" s="9"/>
       <c r="C40" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="D40" s="13" t="s">
         <v>102</v>
-      </c>
-      <c r="D40" s="13" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" s="9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -1835,10 +1839,10 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B43" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C43" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
php 7.2.9 openssl 1.1.0i memcached 1.5.10 libexpat 2.2.6
</commit_message>
<xml_diff>
--- a/src-version.xlsx
+++ b/src-version.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="110">
   <si>
     <t>https://github.com/apache/apr.git</t>
   </si>
@@ -74,9 +74,6 @@
   </si>
   <si>
     <t>https://github.com/libexpat/libexpat.git</t>
-  </si>
-  <si>
-    <t>R_2_2_5</t>
   </si>
   <si>
     <t>https://github.com/GNOME/libxml2.git</t>
@@ -150,12 +147,6 @@
     <t>1.3.2</t>
   </si>
   <si>
-    <t>OpenSSL_1_1_0h</t>
-  </si>
-  <si>
-    <t>0327 OpenSSL_1_1_0g =&gt; OpenSSL_1_1_0h</t>
-  </si>
-  <si>
     <t>https://github.com/apache/subversion</t>
   </si>
   <si>
@@ -220,9 +211,6 @@
   </si>
   <si>
     <t>msvc15 / msvc15-2.9.8</t>
-  </si>
-  <si>
-    <t>msvc15 / msvc15-OpenSSL_1_1_0h</t>
   </si>
   <si>
     <t>msvc15 : bugfix</t>
@@ -288,16 +276,6 @@
     <t>0303 1.0.2 =&gt; 1.0.3
 0411 1.0.3 =&gt; 1.0.4
 0630 1.0.4 =&gt; 1.0.5</t>
-  </si>
-  <si>
-    <t>1.5.9</t>
-  </si>
-  <si>
-    <t>msvc15 / msvc15-1.5.9</t>
-  </si>
-  <si>
-    <t>0612 : 1.5.7 =&gt; 1.5.8
-0724 : 1.5.8 =&gt; 1.5.9</t>
   </si>
   <si>
     <t>0327 master =&gt; php-sdk-2.1.3beta1
@@ -310,7 +288,88 @@
     <t>php-sdk-2.1.7</t>
   </si>
   <si>
-    <t>7.2.8</t>
+    <t>0206 curl-7_57_0 =&gt; curl-7_58_0
+0321 curl-7_58_0 =&gt; curl-7_59_0
+0724 curl-7_61_0</t>
+  </si>
+  <si>
+    <t>curl-7_61_0</t>
+  </si>
+  <si>
+    <t>2.4.34</t>
+  </si>
+  <si>
+    <t>msvc15 / msvc15-2.4.34</t>
+  </si>
+  <si>
+    <t>trunk</t>
+  </si>
+  <si>
+    <t>* 0328 - tag 1.3.9 KO (MSVC 14.1 existe pas)
+0517 : msvc15-1.3.9 from tag 1.3.9
+0517 : trunk ko (openssl runtime cpu)
+0724 : trunk</t>
+  </si>
+  <si>
+    <t>3.24.0</t>
+  </si>
+  <si>
+    <t>1.10.2</t>
+  </si>
+  <si>
+    <t>0328 1.10.0-rc1
+0410 1.10.0-rc1 =&gt; 1.10.0-rc2
+0411 1.10.0-rc2 =&gt; 1.10.0
+0724 : 1.10.2</t>
+  </si>
+  <si>
+    <t>0724 : 3.24.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> * 0301
+0803 2.6.1</t>
+  </si>
+  <si>
+    <t>2.6.1</t>
+  </si>
+  <si>
+    <t>1.1.16</t>
+  </si>
+  <si>
+    <t>0321 : master =&gt; 1.1.10
+0612 : 1.1.10 =&gt; 1.1.12
+0630 : 1.1.12 =&gt; 1.1.15
+0809 : 1.1.15 =&gt; 1.1.16</t>
+  </si>
+  <si>
+    <t>0816 R_2-2-5 =&gt; R_2_2_6</t>
+  </si>
+  <si>
+    <t>R_2_2_6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0612 : 1.5.7 =&gt; 1.5.8
+0724 : 1.5.8 =&gt; 1.5.9
+0816 : 1.5.9 =&gt; 1.5.10 </t>
+  </si>
+  <si>
+    <t>1.5.10</t>
+  </si>
+  <si>
+    <t>msvc15 / msvc15-1.5.10</t>
+  </si>
+  <si>
+    <t>0327 OpenSSL_1_1_0g =&gt; OpenSSL_1_1_0h
+0816 OpenSSL_1_1_0h =&gt; OpenSSL_1_1_0i</t>
+  </si>
+  <si>
+    <t>OpenSSL_1_1_0i</t>
+  </si>
+  <si>
+    <t>msvc15 / msvc15-OpenSSL_1_1_0i</t>
+  </si>
+  <si>
+    <t>7.2.9</t>
   </si>
   <si>
     <t xml:space="preserve"> * 0301
@@ -318,61 +377,8 @@
 0425 7.2.5
 0612 7.2.6
 0630 7.2.7
-0724 7.2.8</t>
-  </si>
-  <si>
-    <t>0206 curl-7_57_0 =&gt; curl-7_58_0
-0321 curl-7_58_0 =&gt; curl-7_59_0
-0724 curl-7_61_0</t>
-  </si>
-  <si>
-    <t>curl-7_61_0</t>
-  </si>
-  <si>
-    <t>2.4.34</t>
-  </si>
-  <si>
-    <t>msvc15 / msvc15-2.4.34</t>
-  </si>
-  <si>
-    <t>trunk</t>
-  </si>
-  <si>
-    <t>* 0328 - tag 1.3.9 KO (MSVC 14.1 existe pas)
-0517 : msvc15-1.3.9 from tag 1.3.9
-0517 : trunk ko (openssl runtime cpu)
-0724 : trunk</t>
-  </si>
-  <si>
-    <t>3.24.0</t>
-  </si>
-  <si>
-    <t>1.10.2</t>
-  </si>
-  <si>
-    <t>0328 1.10.0-rc1
-0410 1.10.0-rc1 =&gt; 1.10.0-rc2
-0411 1.10.0-rc2 =&gt; 1.10.0
-0724 : 1.10.2</t>
-  </si>
-  <si>
-    <t>0724 : 3.24.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> * 0301
-0803 2.6.1</t>
-  </si>
-  <si>
-    <t>2.6.1</t>
-  </si>
-  <si>
-    <t>1.1.16</t>
-  </si>
-  <si>
-    <t>0321 : master =&gt; 1.1.10
-0612 : 1.1.10 =&gt; 1.1.12
-0630 : 1.1.12 =&gt; 1.1.15
-0809 : 1.1.15 =&gt; 1.1.16</t>
+0724 7.2.8
+0816 7.2.9</t>
   </si>
 </sst>
 </file>
@@ -1282,7 +1288,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1292,8 +1298,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1310,7 +1316,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>1</v>
@@ -1323,7 +1329,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>3</v>
@@ -1333,13 +1339,13 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>34</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="9"/>
@@ -1350,10 +1356,10 @@
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="3" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="E4" s="9"/>
     </row>
@@ -1362,7 +1368,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>6</v>
@@ -1378,10 +1384,10 @@
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="3" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="E6" s="9"/>
     </row>
@@ -1390,13 +1396,13 @@
         <v>9</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E7" s="9"/>
     </row>
@@ -1418,7 +1424,7 @@
         <v>13</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>14</v>
@@ -1447,70 +1453,72 @@
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D11" s="2"/>
+        <v>101</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>100</v>
+      </c>
       <c r="E11" s="9"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>6</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E12" s="9"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>43</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="9"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C14" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>38</v>
       </c>
       <c r="E14" s="9"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>22</v>
-      </c>
-      <c r="B15" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>23</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="9"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B16" s="9"/>
       <c r="C16" s="2" t="s">
@@ -1522,63 +1530,63 @@
     </row>
     <row r="17" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B17" s="6"/>
       <c r="C17" s="6" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E17" s="9"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D18" s="8"/>
       <c r="E18" s="9" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="B19" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>41</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="9" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B20" s="6"/>
       <c r="C20" s="6" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="E20" s="9"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
@@ -1587,37 +1595,37 @@
     </row>
     <row r="22" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E22" s="9"/>
+    </row>
+    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B22" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="E22" s="9"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="B23" s="11" t="s">
-        <v>68</v>
+        <v>107</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>45</v>
+        <v>106</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>105</v>
       </c>
       <c r="E23" s="9"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" s="2" t="s">
@@ -1627,12 +1635,12 @@
         <v>7</v>
       </c>
       <c r="E24" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="2" t="s">
@@ -1643,11 +1651,11 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" s="9"/>
@@ -1658,115 +1666,115 @@
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
     </row>
-    <row r="28" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="2" t="s">
-        <v>93</v>
+        <v>108</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>94</v>
+        <v>109</v>
       </c>
       <c r="E28" s="9"/>
     </row>
     <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" s="2" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="E29" s="9"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="E31" s="9"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D32" s="2"/>
       <c r="E32" s="9"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C33" s="9" t="s">
         <v>6</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E33" s="9"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C34" s="9" t="s">
         <v>6</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E34" s="9"/>
     </row>
     <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B35" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="C35" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="B35" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="C35" s="9" t="s">
-        <v>85</v>
-      </c>
       <c r="D35" s="5" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E35" s="9"/>
     </row>
@@ -1776,18 +1784,18 @@
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
     </row>
-    <row r="37" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>89</v>
+        <v>104</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>88</v>
+        <v>103</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>90</v>
+        <v>102</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -1798,38 +1806,38 @@
     </row>
     <row r="39" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" s="2" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B40" s="9"/>
       <c r="C40" s="9" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="D40" s="13" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" s="9" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -1840,10 +1848,10 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B43" s="11" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C43" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
update pcre git repo fix old stuff for jemalloc
</commit_message>
<xml_diff>
--- a/src-version.xlsx
+++ b/src-version.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="114">
   <si>
     <t>https://github.com/apache/apr.git</t>
   </si>
@@ -100,9 +100,6 @@
     <t>https://github.com/openssl/openssl.git</t>
   </si>
   <si>
-    <t>https://github.com/luvit/pcre.git</t>
-  </si>
-  <si>
     <t>https://github.com/madler/zlib.git</t>
   </si>
   <si>
@@ -116,9 +113,6 @@
   </si>
   <si>
     <t>1.2.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 8.41 with JIT, SUPPORT_UTF, SUPPORT_UNICODE_PROPERTIES, REBUILD_CHARTABLES </t>
   </si>
   <si>
     <t xml:space="preserve"> * 0301</t>
@@ -181,9 +175,6 @@
   </si>
   <si>
     <t>https://www.sqlite.org/download.html</t>
-  </si>
-  <si>
-    <t>v1.31.1</t>
   </si>
   <si>
     <t>msvc15 / msvc15-1.2.2</t>
@@ -380,6 +371,27 @@
 0630 php-sdk-2.1.7beta1
 0724 php-sdk-2.1.7
 0820 php-sdk-2.1.8</t>
+  </si>
+  <si>
+    <t>v1.32</t>
+  </si>
+  <si>
+    <t>v1.2.11</t>
+  </si>
+  <si>
+    <t>0821  8.43-RC1 (master)</t>
+  </si>
+  <si>
+    <t>https://github.com/svn2github/pcre.git</t>
+  </si>
+  <si>
+    <t>5.2.4 apachelounge</t>
+  </si>
+  <si>
+    <t>8.42 apachelounge</t>
+  </si>
+  <si>
+    <t>2.2.5 apachelounge</t>
   </si>
 </sst>
 </file>
@@ -1289,7 +1301,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1299,8 +1311,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1317,7 +1329,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>1</v>
@@ -1330,7 +1342,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>3</v>
@@ -1340,13 +1352,13 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>32</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>33</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="9"/>
@@ -1357,10 +1369,10 @@
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E4" s="9"/>
     </row>
@@ -1369,7 +1381,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>6</v>
@@ -1385,10 +1397,10 @@
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E6" s="9"/>
     </row>
@@ -1397,13 +1409,13 @@
         <v>9</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E7" s="9"/>
     </row>
@@ -1425,7 +1437,7 @@
         <v>13</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>14</v>
@@ -1453,38 +1465,40 @@
         <v>19</v>
       </c>
       <c r="B11" s="2"/>
-      <c r="C11" s="3" t="s">
-        <v>99</v>
+      <c r="C11" s="4" t="s">
+        <v>96</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="E11" s="9"/>
+        <v>95</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>6</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E12" s="9"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="9"/>
@@ -1494,13 +1508,13 @@
         <v>20</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E14" s="9"/>
     </row>
@@ -1509,13 +1523,15 @@
         <v>21</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>22</v>
       </c>
       <c r="D15" s="2"/>
-      <c r="E15" s="9"/>
+      <c r="E15" s="4" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
@@ -1535,41 +1551,41 @@
       </c>
       <c r="B17" s="6"/>
       <c r="C17" s="6" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E17" s="9"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D18" s="8"/>
       <c r="E18" s="9" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="9" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -1578,16 +1594,16 @@
       </c>
       <c r="B20" s="6"/>
       <c r="C20" s="6" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E20" s="9"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
@@ -1599,13 +1615,13 @@
         <v>26</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>55</v>
+        <v>107</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E22" s="9"/>
     </row>
@@ -1614,49 +1630,49 @@
         <v>27</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E23" s="9"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>28</v>
+        <v>110</v>
       </c>
       <c r="B24" s="2"/>
-      <c r="C24" s="2" t="s">
+      <c r="C24" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E24" s="9" t="s">
-        <v>34</v>
+        <v>109</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B25" s="2"/>
-      <c r="C25" s="2" t="s">
-        <v>6</v>
+      <c r="C25" s="3" t="s">
+        <v>108</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" s="9"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" s="9"/>
@@ -1669,113 +1685,113 @@
     </row>
     <row r="28" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="E28" s="9"/>
     </row>
     <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E29" s="9"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="E31" s="9"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D32" s="2"/>
       <c r="E32" s="9"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C33" s="9" t="s">
         <v>6</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E33" s="9"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C34" s="9" t="s">
         <v>6</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E34" s="9"/>
     </row>
     <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B35" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="B35" s="11" t="s">
-        <v>80</v>
-      </c>
       <c r="C35" s="9" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E35" s="9"/>
     </row>
@@ -1787,16 +1803,16 @@
     </row>
     <row r="37" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -1807,38 +1823,38 @@
     </row>
     <row r="39" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B40" s="9"/>
       <c r="C40" s="9" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D40" s="13" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="D41" s="9" t="s">
         <v>90</v>
-      </c>
-      <c r="D41" s="9" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -1849,10 +1865,10 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B43" s="11" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C43" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
nghhtp2 1.34 svn 1.10.3
</commit_message>
<xml_diff>
--- a/src-version.xlsx
+++ b/src-version.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\msvc.lan\c$\httpd-sdk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5731CC8A-6187-4920-922B-D323E992ED33}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD851D26-E5A5-4A4B-B097-B6E9BBF4D845}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -254,15 +254,6 @@
     <t>3.24.0</t>
   </si>
   <si>
-    <t>1.10.2</t>
-  </si>
-  <si>
-    <t>0328 1.10.0-rc1
-0410 1.10.0-rc1 =&gt; 1.10.0-rc2
-0411 1.10.0-rc2 =&gt; 1.10.0
-0724 : 1.10.2</t>
-  </si>
-  <si>
     <t>0724 : 3.24.0</t>
   </si>
   <si>
@@ -339,19 +330,6 @@
   </si>
   <si>
     <t>1.11.0</t>
-  </si>
-  <si>
-    <t>msvc15 / msvc15-v1.33.0</t>
-  </si>
-  <si>
-    <t>v1.33</t>
-  </si>
-  <si>
-    <t>0206 master =&gt; v1.30.0
-0301 v1.30.0 =&gt; v1.31.0
-0415 v1.31.0 =&gt; v1.31.1
-0514 v1.32.0
-0911 v1.33.0</t>
   </si>
   <si>
     <t>7.2.10</t>
@@ -409,6 +387,30 @@
 0303 2.4.30 =&gt; 2.4.31
 0321 2.4.31 =&gt; 2.4.33
 0930 =&gt; 2.4.35</t>
+  </si>
+  <si>
+    <t>msvc15 / msvc15-v1.34.0</t>
+  </si>
+  <si>
+    <t>v1.34</t>
+  </si>
+  <si>
+    <t>0206 master =&gt; v1.30.0
+0301 v1.30.0 =&gt; v1.31.0
+0415 v1.31.0 =&gt; v1.31.1
+0514 v1.32.0
+1006 v1.34.0
+0911 v1.33.0</t>
+  </si>
+  <si>
+    <t>1.10.3</t>
+  </si>
+  <si>
+    <t>0328 1.10.0-rc1
+0410 1.10.0-rc1 =&gt; 1.10.0-rc2
+0411 1.10.0-rc2 =&gt; 1.10.0
+0724 1.10.2
+1006 1.10.3</t>
   </si>
 </sst>
 </file>
@@ -1328,8 +1330,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A12" sqref="A11:A12"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1346,13 +1348,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E1" s="9"/>
     </row>
@@ -1388,10 +1390,10 @@
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="3" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="E4" s="9"/>
     </row>
@@ -1419,7 +1421,7 @@
         <v>72</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E6" s="9"/>
     </row>
@@ -1428,13 +1430,13 @@
         <v>8</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="E7" s="9"/>
     </row>
@@ -1485,13 +1487,13 @@
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1549,7 +1551,7 @@
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -1570,10 +1572,10 @@
       </c>
       <c r="B17" s="6"/>
       <c r="C17" s="6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E17" s="9"/>
     </row>
@@ -1613,10 +1615,10 @@
       </c>
       <c r="B20" s="6"/>
       <c r="C20" s="6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E20" s="9"/>
     </row>
@@ -1629,18 +1631,18 @@
       <c r="D21" s="6"/>
       <c r="E21" s="9"/>
     </row>
-    <row r="22" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="E22" s="9"/>
     </row>
@@ -1650,26 +1652,26 @@
       </c>
       <c r="B23" s="9"/>
       <c r="C23" s="3" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="E23" s="9"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1677,10 +1679,10 @@
         <v>27</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" s="9"/>
@@ -1708,10 +1710,10 @@
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="2" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="E28" s="9"/>
     </row>
@@ -1721,10 +1723,10 @@
       </c>
       <c r="B29" s="2"/>
       <c r="C29" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E29" s="9"/>
     </row>
@@ -1751,10 +1753,10 @@
       </c>
       <c r="B31" s="2"/>
       <c r="C31" s="2" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="E31" s="9"/>
     </row>
@@ -1825,13 +1827,13 @@
         <v>40</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -1840,16 +1842,16 @@
       <c r="C38" s="15"/>
       <c r="D38" s="15"/>
     </row>
-    <row r="39" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>39</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" s="2" t="s">
-        <v>76</v>
+        <v>113</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>77</v>
+        <v>114</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -1873,7 +1875,7 @@
         <v>75</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
httpd 2.4.36 mod_h2 1.11.3 php 7.2.11
</commit_message>
<xml_diff>
--- a/src-version.xlsx
+++ b/src-version.xlsx
@@ -273,17 +273,6 @@
     <t>R_2_2_6</t>
   </si>
   <si>
-    <t xml:space="preserve">0612 : 1.5.7 =&gt; 1.5.8
-0724 : 1.5.8 =&gt; 1.5.9
-0816 : 1.5.9 =&gt; 1.5.10 </t>
-  </si>
-  <si>
-    <t>1.5.10</t>
-  </si>
-  <si>
-    <t>msvc15 / msvc15-1.5.10</t>
-  </si>
-  <si>
     <t>v1.2.11</t>
   </si>
   <si>
@@ -317,7 +306,75 @@
 0911 curl-7_61_0 =&gt; curl-7_61_1</t>
   </si>
   <si>
-    <t>7.2.10</t>
+    <t>msvc15 / msvc15-v1.2.11</t>
+  </si>
+  <si>
+    <t>OpenSSL_1_1_1</t>
+  </si>
+  <si>
+    <t>0327 OpenSSL_1_1_0g =&gt; OpenSSL_1_1_0h
+0816 OpenSSL_1_1_0h =&gt; OpenSSL_1_1_0i
+0912 OpenSSL_1_1_1</t>
+  </si>
+  <si>
+    <t>v1.0.6</t>
+  </si>
+  <si>
+    <t>0303 1.0.2 =&gt; 1.0.3
+0411 1.0.3 =&gt; 1.0.4
+0630 1.0.4 =&gt; 1.0.5
+0930 1.0.6</t>
+  </si>
+  <si>
+    <t>php-sdk-2.1.9</t>
+  </si>
+  <si>
+    <t>0327 master =&gt; php-sdk-2.1.3beta1
+0502 php-sdk-2.1.4
+0514 php-sdk-2.1.5
+0630 php-sdk-2.1.7beta1
+0724 php-sdk-2.1.7
+0820 php-sdk-2.1.8
+0930 php-sdk-2.1.9</t>
+  </si>
+  <si>
+    <t>msvc15 / msvc15-v1.34.0</t>
+  </si>
+  <si>
+    <t>v1.34</t>
+  </si>
+  <si>
+    <t>0206 master =&gt; v1.30.0
+0301 v1.30.0 =&gt; v1.31.0
+0415 v1.31.0 =&gt; v1.31.1
+0514 v1.32.0
+1006 v1.34.0
+0911 v1.33.0</t>
+  </si>
+  <si>
+    <t>1.10.3</t>
+  </si>
+  <si>
+    <t>0328 1.10.0-rc1
+0410 1.10.0-rc1 =&gt; 1.10.0-rc2
+0411 1.10.0-rc2 =&gt; 1.10.0
+0724 1.10.2
+1006 1.10.3</t>
+  </si>
+  <si>
+    <t>msvc15 / msvc15-1.5.11</t>
+  </si>
+  <si>
+    <t>1.5.11</t>
+  </si>
+  <si>
+    <t>0612 : 1.5.7 =&gt; 1.5.8
+0724 : 1.5.8 =&gt; 1.5.9
+0816 : 1.5.9 =&gt; 1.5.10
+1011 : 1.5.11</t>
+  </si>
+  <si>
+    <t>7.2.11</t>
   </si>
   <si>
     <t xml:space="preserve"> * 0301
@@ -327,85 +384,32 @@
 0630 7.2.7
 0724 7.2.8
 0816 7.2.9
-0911 7.2.10</t>
-  </si>
-  <si>
-    <t>msvc15 / msvc15-v1.2.11</t>
-  </si>
-  <si>
-    <t>OpenSSL_1_1_1</t>
-  </si>
-  <si>
-    <t>0327 OpenSSL_1_1_0g =&gt; OpenSSL_1_1_0h
-0816 OpenSSL_1_1_0h =&gt; OpenSSL_1_1_0i
-0912 OpenSSL_1_1_1</t>
-  </si>
-  <si>
-    <t>v1.0.6</t>
-  </si>
-  <si>
-    <t>0303 1.0.2 =&gt; 1.0.3
-0411 1.0.3 =&gt; 1.0.4
-0630 1.0.4 =&gt; 1.0.5
-0930 1.0.6</t>
-  </si>
-  <si>
-    <t>php-sdk-2.1.9</t>
-  </si>
-  <si>
-    <t>0327 master =&gt; php-sdk-2.1.3beta1
-0502 php-sdk-2.1.4
-0514 php-sdk-2.1.5
-0630 php-sdk-2.1.7beta1
-0724 php-sdk-2.1.7
-0820 php-sdk-2.1.8
-0930 php-sdk-2.1.9</t>
-  </si>
-  <si>
-    <t>2.4.35</t>
-  </si>
-  <si>
-    <t>msvc15 / msvc15-2.4.35</t>
+0911 7.2.10
+1011 7.2.11</t>
+  </si>
+  <si>
+    <t>msvc15 / msvc15-2.4.36</t>
+  </si>
+  <si>
+    <t>2.4.36</t>
   </si>
   <si>
     <t>0219 2.4.29 =&gt; 2.4.30
 0303 2.4.30 =&gt; 2.4.31
 0321 2.4.31 =&gt; 2.4.33
-0930 =&gt; 2.4.35</t>
-  </si>
-  <si>
-    <t>msvc15 / msvc15-v1.34.0</t>
-  </si>
-  <si>
-    <t>v1.34</t>
-  </si>
-  <si>
-    <t>0206 master =&gt; v1.30.0
-0301 v1.30.0 =&gt; v1.31.0
-0415 v1.31.0 =&gt; v1.31.1
-0514 v1.32.0
-1006 v1.34.0
-0911 v1.33.0</t>
-  </si>
-  <si>
-    <t>1.10.3</t>
-  </si>
-  <si>
-    <t>0328 1.10.0-rc1
-0410 1.10.0-rc1 =&gt; 1.10.0-rc2
-0411 1.10.0-rc2 =&gt; 1.10.0
-0724 1.10.2
-1006 1.10.3</t>
-  </si>
-  <si>
-    <t>1.11.1</t>
+0930 =&gt; 2.4.35
+1011 =&gt; 2.4.36</t>
+  </si>
+  <si>
+    <t>1.11.3</t>
   </si>
   <si>
     <t>0212 master =&gt; 1.10.16
 0410 1.10.17 =&gt; 1.10.17
 0502 1.10.20
 0911 : 1.11.0
-1009 : 1.11.1</t>
+1009 : 1.11.1
+1011 : 1.11.3</t>
   </si>
 </sst>
 </file>
@@ -1315,7 +1319,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1325,8 +1329,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1343,13 +1347,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E1" s="9"/>
     </row>
@@ -1385,10 +1389,10 @@
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="3" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="E4" s="9"/>
     </row>
@@ -1416,22 +1420,22 @@
         <v>72</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E6" s="9"/>
     </row>
-    <row r="7" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="E7" s="9"/>
     </row>
@@ -1488,7 +1492,7 @@
         <v>81</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1546,7 +1550,7 @@
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="4" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -1561,7 +1565,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>23</v>
       </c>
@@ -1631,13 +1635,13 @@
         <v>25</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="E22" s="9"/>
     </row>
@@ -1647,26 +1651,26 @@
       </c>
       <c r="B23" s="9"/>
       <c r="C23" s="3" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E23" s="9"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D24" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E24" s="4" t="s">
         <v>87</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1674,10 +1678,10 @@
         <v>27</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" s="9"/>
@@ -1699,16 +1703,16 @@
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
     </row>
-    <row r="28" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="135" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="2" t="s">
-        <v>96</v>
+        <v>108</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>97</v>
+        <v>109</v>
       </c>
       <c r="E28" s="9"/>
     </row>
@@ -1748,10 +1752,10 @@
       </c>
       <c r="B31" s="2"/>
       <c r="C31" s="2" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="E31" s="9"/>
     </row>
@@ -1817,18 +1821,18 @@
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
     </row>
-    <row r="37" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>40</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>85</v>
+        <v>105</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>84</v>
+        <v>106</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>83</v>
+        <v>107</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -1843,10 +1847,10 @@
       </c>
       <c r="B39" s="2"/>
       <c r="C39" s="2" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="60" x14ac:dyDescent="0.25">

</xml_diff>